<commit_message>
xls changed in new branch
</commit_message>
<xml_diff>
--- a/b.xlsx
+++ b/b.xlsx
@@ -24,14 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>n</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
     <t>surname</t>
   </si>
   <si>
@@ -39,6 +36,15 @@
   </si>
   <si>
     <t>dsa</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>ew</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -357,10 +363,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -370,10 +376,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -381,10 +387,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -392,10 +398,21 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
xls changed in new branch 2
</commit_message>
<xml_diff>
--- a/b.xlsx
+++ b/b.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t>n</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>s</t>
+  </si>
+  <si>
+    <t>da</t>
   </si>
 </sst>
 </file>
@@ -363,10 +366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -415,6 +418,17 @@
         <v>6</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>